<commit_message>
Añadido nivel de fermi en el excel
</commit_message>
<xml_diff>
--- a/datos/2traps.xlsx
+++ b/datos/2traps.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">E (eV)</t>
   </si>
@@ -254,6 +254,9 @@
       <t xml:space="preserve">-3)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Ef</t>
+  </si>
 </sst>
 </file>
 
@@ -381,7 +384,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,6 +446,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -571,10 +578,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q999"/>
+  <dimension ref="A1:R999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -647,6 +654,9 @@
       <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
@@ -700,6 +710,9 @@
       </c>
       <c r="Q2" s="12" t="n">
         <v>0</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>2.7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -753,18 +766,18 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
       <c r="N6" s="3"/>
       <c r="O6" s="2"/>
     </row>
@@ -774,12 +787,12 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13"/>
@@ -787,40 +800,40 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="23"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O14" s="1"/>
@@ -832,20 +845,20 @@
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1841,7 +1854,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1864,7 +1877,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="R1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>